<commit_message>
Updating new data files
</commit_message>
<xml_diff>
--- a/DLS_Plots/20240119_DLS_DIPLibrary_NP10_finalrepeat_01XPBS copy.xlsx
+++ b/DLS_Plots/20240119_DLS_DIPLibrary_NP10_finalrepeat_01XPBS copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mines0-my.sharepoint.com/personal/aryellewright_mines_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/DLS_Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{9AB7F2A3-AE04-4848-8DC8-337BF047FE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE02F23D-455E-434D-9EE3-9B962AF2AD88}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF7D3D8-01D1-7046-AA55-D5D0D6963079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1660" windowWidth="24640" windowHeight="14320" xr2:uid="{2E69A96F-4750-1745-BC8E-14D773EF51E6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Polymer</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>G3</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -415,7 +421,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,7 +442,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>267.57</v>
@@ -447,7 +453,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>3259.7999999999997</v>

</xml_diff>